<commit_message>
updated map with parts that have been completed
</commit_message>
<xml_diff>
--- a/conceptualmap-tlk.xlsx
+++ b/conceptualmap-tlk.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16720" tabRatio="500" activeTab="1"/>
@@ -64,9 +64,6 @@
     <t>tag each sentence that is entered during this session with: language name, location of data collection, user name</t>
   </si>
   <si>
-    <t>database structure that will record each sentence that is entered and all of the corresponding metadata</t>
-  </si>
-  <si>
     <t>User starts a new session and enters the following info: language name, where the langauge is spoken locally, where the data was collected (each data set corresponds to a different session)</t>
   </si>
   <si>
@@ -94,33 +91,15 @@
     <t>need function that asks user to type phrasal consitutents then select phrase label using drop-down menu</t>
   </si>
   <si>
-    <t>the program adds each phrase to a list according to its phrase type</t>
-  </si>
-  <si>
     <t>How to assist users in making the right phrasal groupings?</t>
   </si>
   <si>
     <t>Provide constituency tests for guidance - this resource should only appear duing the level 2 tagging stage</t>
   </si>
   <si>
-    <t>what will it take to do this in the app? Opening a new page?</t>
-  </si>
-  <si>
     <t>the program generates a phrase structure rule for the sentence according to the phrasal grouping provided by the user; the program presents the phrase-structure rule to the user and adds it to the grammar for the session (a list of phrase structure rules that can account for the data entered during the session)</t>
   </si>
   <si>
-    <t>need separate list to store phrase types and tokens for each session</t>
-  </si>
-  <si>
-    <t>need separate list to store lexicon for each session -- part-of-speech types and tokens</t>
-  </si>
-  <si>
-    <t>need function to assign phrases to different lists according their phrase type</t>
-  </si>
-  <si>
-    <t>need function that adds word and part-of-speech tag to a list</t>
-  </si>
-  <si>
     <t>need function to general PS rule based on user's phrase divisions and their order in the sentence</t>
   </si>
   <si>
@@ -164,9 +143,6 @@
   </si>
   <si>
     <t>intro page with user login; fields for entering session info: 1. language name; 2. where spoken; 3. data collection context</t>
-  </si>
-  <si>
-    <t>need functions that will ask for user/session data and create a new data set based on this info</t>
   </si>
   <si>
     <t>getSentence(): function in WordTag.py</t>
@@ -484,13 +460,7 @@
     </r>
   </si>
   <si>
-    <t>the program presents the full sentence with part-of-speech tags on each word to the user and asks if the info is correct</t>
-  </si>
-  <si>
     <t>if the user answers "yes"</t>
-  </si>
-  <si>
-    <t>if the user answers "no"</t>
   </si>
   <si>
     <r>
@@ -530,9 +500,6 @@
     </r>
   </si>
   <si>
-    <t>the program adds the word:part-of-speech pair contents of the dictionary to a "vocabulary" database for the session; then displays the same sentence to the user for Level 2 analysis</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">in </t>
     </r>
@@ -621,19 +588,109 @@
       <t>; there needs to be another function that stores the dictionary contents in a "vocabulary" database</t>
     </r>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">need function that adds word and part-of-speech tag to a table: in lev1main.py </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pos_confirm(pos_tags):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+ for word in pos_tags:
+            dict_cur.execute("INSERT INTO words(word, pos, language) VALUES (%s,%s, %s)",(word, pos_tags[word],"english"))
+</t>
+    </r>
+  </si>
+  <si>
+    <t>need separate table to store lexicon for each session -- part-of-speech types and tokens (tables created at 2/18/15 mtg.)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">the program presents the full sentence with part-of-speech tags on each word to the user and asks if the info is correct - in lev1main.py, function </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pos_confirm(pos_tags):</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">need functions that will ask for user/session data and create a new data set based on this info - in lev1main.py #connect to psql database
+urlparse.uses_netloc.append("postgres")
+url = urlparse.urlparse("")
+conn = psycopg2.connect(
+database=url.path[1:],
+user=url.username,
+password=url.password,
+host=url.hostname,
+port=url.port
+)
+conn.set_session(autocommit=True)
+dict_cur = conn.cursor(cursor_factory=psycopg2.extras.DictCursor)
+</t>
+  </si>
+  <si>
+    <t>database structure that will record each sentence that is entered and all of the corresponding metadata: tables created at 2/18/15 mtg.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">if the user answers "no": loops back through </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>levonemain()</t>
+    </r>
+  </si>
+  <si>
+    <t>the program adds the word:part-of-speech pair contents of the dictionary to a "vocabulary" table for the session; then displays the same sentence to the user for Level 2 analysis</t>
+  </si>
+  <si>
+    <t>what will it take to do this in the app? Opening a new page? I think that having the guides and data entry field on the same page would be best</t>
+  </si>
+  <si>
+    <t xml:space="preserve">need function to assign phrase:phrase tag key-value pairs from each sentence to a "phrase-level-info" table </t>
+  </si>
+  <si>
+    <t>Do we need separate tables to store phrase types and tokens for each session? I don't think so, but we do need to be able to operate on each level independently--some functions will only need info about phrase types, other functions will need info about the tokens that have been recorded for each type</t>
+  </si>
+  <si>
+    <t>the program adds each phrase and it's phrase label to a table in the database</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -806,120 +863,122 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="111">
+  <cellStyleXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -927,7 +986,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -936,7 +995,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -951,16 +1010,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -972,19 +1031,22 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="111">
+  <cellStyles count="113">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -1041,6 +1103,7 @@
     <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
@@ -1095,6 +1158,7 @@
     <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2900,89 +2964,89 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="18" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="B12" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B13" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="18" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="19" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B19" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -2990,7 +3054,7 @@
         <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -2998,34 +3062,34 @@
     </row>
     <row r="22" spans="1:2" ht="30">
       <c r="A22" s="20" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="19" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B24" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="19" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="19" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B26" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -3043,10 +3107,10 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="18" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3079,7 +3143,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
@@ -3095,7 +3159,7 @@
     </row>
     <row r="4" spans="1:12" ht="136" thickBot="1">
       <c r="B4" s="14" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C4" s="4"/>
       <c r="F4" s="11" t="s">
@@ -3113,20 +3177,20 @@
     </row>
     <row r="6" spans="1:12" ht="152" customHeight="1">
       <c r="B6" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="8" t="s">
-        <v>48</v>
+      <c r="J6" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="L6" s="8" t="s">
-        <v>14</v>
+        <v>40</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="29" customHeight="1">
@@ -3134,10 +3198,10 @@
     </row>
     <row r="8" spans="1:12" ht="105">
       <c r="B8" s="2" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="K8" s="8" t="s">
         <v>7</v>
@@ -3150,20 +3214,20 @@
     </row>
     <row r="10" spans="1:12" ht="225">
       <c r="B10" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="L10" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="J10" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="37" customHeight="1">
@@ -3174,47 +3238,47 @@
     </row>
     <row r="12" spans="1:12" ht="120">
       <c r="B12" s="2" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="30" customHeight="1"/>
+    <row r="14" spans="1:12" ht="270">
+      <c r="C14" s="4"/>
+      <c r="D14" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="F12" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" ht="30" customHeight="1"/>
-    <row r="14" spans="1:12" ht="255">
-      <c r="C14" s="4"/>
-      <c r="D14" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>93</v>
+      <c r="F14" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="J14" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="L14" s="8" t="s">
-        <v>30</v>
+        <v>79</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="34" customHeight="1">
       <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:12" ht="58" customHeight="1">
-      <c r="B16" s="9" t="s">
-        <v>90</v>
+      <c r="B16" s="22" t="s">
+        <v>88</v>
       </c>
       <c r="C16" s="4"/>
     </row>
@@ -3222,48 +3286,48 @@
       <c r="D17" s="5"/>
     </row>
     <row r="18" spans="2:12" ht="61" customHeight="1">
-      <c r="B18" s="9" t="s">
-        <v>89</v>
+      <c r="B18" s="22" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="2:12" ht="37" customHeight="1"/>
     <row r="20" spans="2:12" ht="134" customHeight="1">
       <c r="B20" s="8" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C20" s="4"/>
-      <c r="D20" s="22" t="s">
-        <v>92</v>
+      <c r="D20" s="23" t="s">
+        <v>89</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H20" s="16" t="s">
-        <v>27</v>
+        <v>90</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K20" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" spans="2:12" ht="37" customHeight="1">
       <c r="D21" s="5"/>
     </row>
-    <row r="22" spans="2:12" ht="97" customHeight="1">
+    <row r="22" spans="2:12" ht="230" customHeight="1">
       <c r="C22" s="4"/>
       <c r="D22" s="8" t="s">
-        <v>24</v>
+        <v>93</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="L22" s="8" t="s">
-        <v>29</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="2:12" ht="37" customHeight="1">
@@ -3273,13 +3337,13 @@
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
       <c r="D24" s="8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="J24" s="8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="L24" s="8" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="2:12" ht="38" customHeight="1">
@@ -3287,17 +3351,17 @@
     </row>
     <row r="26" spans="2:12" ht="185" customHeight="1">
       <c r="B26" s="8" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="8" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="J26" s="8" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="2:12" ht="28" customHeight="1">
@@ -3306,7 +3370,7 @@
     <row r="28" spans="2:12" ht="94" customHeight="1">
       <c r="C28" s="4"/>
       <c r="D28" s="8" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="L28" s="4"/>
     </row>
@@ -3317,20 +3381,20 @@
     </row>
     <row r="30" spans="2:12" ht="177" customHeight="1">
       <c r="B30" s="9" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="17" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="K30" s="8" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="2:12" ht="36" customHeight="1">
@@ -3340,7 +3404,7 @@
     </row>
     <row r="32" spans="2:12" ht="153" customHeight="1">
       <c r="D32" s="9" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="4:10" ht="39" customHeight="1">
@@ -3348,7 +3412,7 @@
     </row>
     <row r="34" spans="4:10" ht="120">
       <c r="D34" s="8" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="F34" s="2" t="s">
         <v>2</v>
@@ -3357,12 +3421,12 @@
         <v>3</v>
       </c>
       <c r="J34" s="8" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="4:10" ht="150">
       <c r="D35" s="10" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="I35" s="1"/>
     </row>

</xml_diff>